<commit_message>
Mistake Corrected in Documents
</commit_message>
<xml_diff>
--- a/Project/Work breakdown structure.xlsx
+++ b/Project/Work breakdown structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ana Carolina Gadelha\IdeaProjects\ganttproject2\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5BE8A0-48B3-45AD-AC32-15CD1798A041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127FB058-03C9-4B39-AFD6-8302ADA58B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33345" yWindow="1575" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>2.2 - Metrics</t>
   </si>
 </sst>
 </file>
@@ -190,7 +193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -371,11 +374,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -398,8 +410,25 @@
     <xf numFmtId="14" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -414,39 +443,34 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -666,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -682,10 +706,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -700,20 +724,20 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="11"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="2">
@@ -730,8 +754,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="25" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2">
@@ -748,8 +772,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="25" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2">
@@ -766,8 +790,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="25" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="2">
@@ -784,8 +808,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="25" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="2">
@@ -802,20 +826,20 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="7">
@@ -832,8 +856,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="7">
@@ -850,8 +874,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="7">
@@ -868,8 +892,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="7">
@@ -886,8 +910,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="7">
@@ -904,8 +928,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="21" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="7">
@@ -922,80 +946,80 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="12">
         <v>44893</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="12">
         <v>44895</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="24" t="s">
+      <c r="A16" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="12">
         <v>44893</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="12">
         <v>44896</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="24" t="s">
+      <c r="A17" s="27"/>
+      <c r="B17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="7">
         <v>44893</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="7">
         <v>44896</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="9"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="9"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="9"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="9"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1977,12 +2001,12 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A9:A15"/>
-    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>